<commit_message>
update analysis and charts
</commit_message>
<xml_diff>
--- a/server/analysis/qualtrics/multiple_choice_charts.xlsx
+++ b/server/analysis/qualtrics/multiple_choice_charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acosc\Documents\GitHub\cs6795-project\server\analysis\qualtrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C948C3-5A35-490A-AD61-8429D3C11637}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B7F3E6-0674-40CB-9A76-0F28308DB081}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="709" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="709" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="2" r:id="rId1"/>
@@ -1292,12 +1292,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx2">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1628,12 +1623,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx2">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1958,12 +1948,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx2">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2276,12 +2261,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx2">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -4758,7 +4738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AF4F6C-3EA1-4FE5-9D69-12AAC2E85E9F}">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -7409,7 +7389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F756EE-3C66-4AA9-8718-04EB56D50E53}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>

</xml_diff>